<commit_message>
Added library, finished Flipdot.xlsx
</commit_message>
<xml_diff>
--- a/Flipdot.xlsx
+++ b/Flipdot.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\eagle\projects\Flipdot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>1. sor GND</t>
   </si>
@@ -150,6 +150,111 @@
   </si>
   <si>
     <t>C1</t>
+  </si>
+  <si>
+    <t>Row 2 L</t>
+  </si>
+  <si>
+    <t>Row 3 L</t>
+  </si>
+  <si>
+    <t>Row 4 L</t>
+  </si>
+  <si>
+    <t>Row 5 L</t>
+  </si>
+  <si>
+    <t>Row 6 L</t>
+  </si>
+  <si>
+    <t>Row 7 L</t>
+  </si>
+  <si>
+    <t>Row 2 H</t>
+  </si>
+  <si>
+    <t>Row 3 H</t>
+  </si>
+  <si>
+    <t>Row 4 H</t>
+  </si>
+  <si>
+    <t>Row 5 H</t>
+  </si>
+  <si>
+    <t>Row 6 H</t>
+  </si>
+  <si>
+    <t>Row 7 H</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>C15</t>
+  </si>
+  <si>
+    <t>C16</t>
+  </si>
+  <si>
+    <t>C17</t>
+  </si>
+  <si>
+    <t>C18</t>
+  </si>
+  <si>
+    <t>C19</t>
+  </si>
+  <si>
+    <t>C20</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>C23</t>
+  </si>
+  <si>
+    <t>C24</t>
   </si>
 </sst>
 </file>
@@ -823,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,296 +1075,401 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="K6" t="s">
+      <c r="E6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="E7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
         <v>1</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C10" s="13">
         <v>21</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D10" s="22" t="s">
         <v>32</v>
-      </c>
-      <c r="K7" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
-        <v>2</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="15">
-        <v>22</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
-        <v>3</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="15">
-        <v>23</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
-        <v>4</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="15">
-        <v>24</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
+        <v>2</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>2</v>
-      </c>
       <c r="C11" s="15">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C12" s="15">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C13" s="15">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
-        <v>8</v>
-      </c>
-      <c r="B14" s="17"/>
+        <v>5</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="C14" s="15">
-        <v>28</v>
-      </c>
-      <c r="D14" s="17"/>
+        <v>25</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
-        <v>9</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>1</v>
       </c>
       <c r="C15" s="15">
-        <v>29</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>8</v>
+        <v>26</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
-        <v>10</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>0</v>
       </c>
       <c r="C16" s="15">
-        <v>30</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>10</v>
+        <v>27</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
-        <v>11</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>13</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B17" s="17"/>
       <c r="C17" s="15">
-        <v>31</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>12</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D17" s="17"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C18" s="15">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C19" s="15">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C20" s="15">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
+        <v>12</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="18" t="s">
-        <v>21</v>
-      </c>
       <c r="C21" s="15">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
+        <v>13</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="15">
+        <v>33</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>16</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="15">
-        <v>36</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C23" s="15">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C24" s="15">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
+        <v>16</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="15">
+        <v>36</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>17</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="15">
+        <v>37</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>18</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="15">
+        <v>38</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
         <v>19</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B28" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C28" s="15">
         <v>39</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D28" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20">
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="20">
         <v>20</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B29" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C29" s="20">
         <v>40</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="D29" s="21" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>